<commit_message>
major updates to transmission data!
</commit_message>
<xml_diff>
--- a/gt_sources/janelia_easi_fish/040624_NT_Summary_List_Jan_Lou.xlsx
+++ b/gt_sources/janelia_easi_fish/040624_NT_Summary_List_Jan_Lou.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abates/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GD/LMBD/Papers/synister/drosophila_neurotransmitters/gt_sources/janelia_easi_fish/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B07F0C12-283F-ED4C-A165-C8B9055E66A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CB3C77-7D20-8D42-B537-C09E69EA3CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="24120" windowHeight="16820" xr2:uid="{9F11D1D6-F0B9-2649-8C33-E08693602A84}"/>
+    <workbookView xWindow="-27260" yWindow="3740" windowWidth="24120" windowHeight="16820" xr2:uid="{9F11D1D6-F0B9-2649-8C33-E08693602A84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="374">
   <si>
     <t>Key:</t>
   </si>
@@ -1176,6 +1176,18 @@
   </si>
   <si>
     <t>** very low expression, and ambigious</t>
+  </si>
+  <si>
+    <t>FB1H=serotonin</t>
+  </si>
+  <si>
+    <t>FB2B=octopamine/tyramine</t>
+  </si>
+  <si>
+    <t>PFR=tyramine</t>
+  </si>
+  <si>
+    <t>FB7K=dopamine</t>
   </si>
 </sst>
 </file>
@@ -2123,15 +2135,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B59386-8207-5A47-BCDE-133FFF6C097D}">
-  <dimension ref="A1:G204"/>
+  <dimension ref="A1:G210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G191" sqref="G191"/>
+    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A207" sqref="A207:A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="28.83203125" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
@@ -5515,6 +5527,26 @@
         <v>333</v>
       </c>
     </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>373</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>